<commit_message>
added petroleum and natural gas legend
</commit_message>
<xml_diff>
--- a/Final Project/data/use_tot_realgdp.xlsx
+++ b/Final Project/data/use_tot_realgdp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\CSEDS\Internet\Data\Consum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellelouie/Documents/Berkeley/2024-2025/STAT 198/stat-198/Final Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9431D3D2-630C-489F-BBAC-2921BF880630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4442FF6B-CC5D-554F-80CC-22728C6E54C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7635" windowWidth="29040" windowHeight="15840" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18700" tabRatio="657" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="7" r:id="rId1"/>
@@ -46,10 +46,21 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1332,42 +1343,42 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="59.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.9140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="4"/>
-    <col min="5" max="5" width="10.4140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="4" customWidth="1"/>
     <col min="6" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1384,7 +1395,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +1412,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1431,7 @@
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1439,30 +1450,30 @@
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -1486,28 +1497,28 @@
   <dimension ref="A1:CW56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="BD22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BL4" sqref="BL4:BL55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" customWidth="1"/>
     <col min="2" max="64" width="11.1640625" style="9" customWidth="1"/>
     <col min="65" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1712,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -1932,7 +1943,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>32</v>
       </c>
@@ -2163,7 +2174,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -2394,7 +2405,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
@@ -2625,7 +2636,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
@@ -2856,7 +2867,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
@@ -3087,7 +3098,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -3318,7 +3329,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
@@ -3549,7 +3560,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>39</v>
       </c>
@@ -3780,7 +3791,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>40</v>
       </c>
@@ -4011,7 +4022,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -4242,7 +4253,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>42</v>
       </c>
@@ -4473,7 +4484,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
@@ -4704,7 +4715,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -4935,7 +4946,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>45</v>
       </c>
@@ -5166,7 +5177,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -5397,7 +5408,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>47</v>
       </c>
@@ -5628,7 +5639,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>48</v>
       </c>
@@ -5859,7 +5870,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>49</v>
       </c>
@@ -6090,7 +6101,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>50</v>
       </c>
@@ -6321,7 +6332,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>51</v>
       </c>
@@ -6552,7 +6563,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>52</v>
       </c>
@@ -6783,7 +6794,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>53</v>
       </c>
@@ -7014,7 +7025,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>54</v>
       </c>
@@ -7245,7 +7256,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>55</v>
       </c>
@@ -7476,7 +7487,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>56</v>
       </c>
@@ -7707,7 +7718,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
@@ -7938,7 +7949,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>58</v>
       </c>
@@ -8169,7 +8180,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>59</v>
       </c>
@@ -8400,7 +8411,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>60</v>
       </c>
@@ -8631,7 +8642,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>61</v>
       </c>
@@ -8862,7 +8873,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>62</v>
       </c>
@@ -9093,7 +9104,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>63</v>
       </c>
@@ -9324,7 +9335,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>64</v>
       </c>
@@ -9555,7 +9566,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>65</v>
       </c>
@@ -9786,7 +9797,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>66</v>
       </c>
@@ -10017,7 +10028,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>67</v>
       </c>
@@ -10248,7 +10259,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>68</v>
       </c>
@@ -10479,7 +10490,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>69</v>
       </c>
@@ -10710,7 +10721,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>70</v>
       </c>
@@ -10941,7 +10952,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>71</v>
       </c>
@@ -11172,7 +11183,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>72</v>
       </c>
@@ -11403,7 +11414,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>73</v>
       </c>
@@ -11634,7 +11645,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>74</v>
       </c>
@@ -11865,7 +11876,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>75</v>
       </c>
@@ -12096,7 +12107,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>76</v>
       </c>
@@ -12327,7 +12338,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>77</v>
       </c>
@@ -12558,7 +12569,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>78</v>
       </c>
@@ -12789,7 +12800,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>79</v>
       </c>
@@ -13020,7 +13031,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>80</v>
       </c>
@@ -13251,7 +13262,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>81</v>
       </c>
@@ -13482,7 +13493,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>82</v>
       </c>
@@ -13713,7 +13724,7 @@
       <c r="CV55" s="10"/>
       <c r="CW55" s="10"/>
     </row>
-    <row r="56" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.2">
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
@@ -13794,28 +13805,28 @@
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AX4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BL55" sqref="BL4:BL55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" style="6" customWidth="1"/>
-    <col min="2" max="64" width="12.4140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" customWidth="1"/>
+    <col min="2" max="64" width="12.33203125" style="9" customWidth="1"/>
     <col min="65" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -14009,7 +14020,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -14166,7 +14177,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>32</v>
       </c>
@@ -14323,7 +14334,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -14480,7 +14491,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
@@ -14637,7 +14648,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
@@ -14794,7 +14805,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
@@ -14951,7 +14962,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -15108,7 +15119,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
@@ -15265,7 +15276,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>39</v>
       </c>
@@ -15422,7 +15433,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>40</v>
       </c>
@@ -15579,7 +15590,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -15736,7 +15747,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>42</v>
       </c>
@@ -15893,7 +15904,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
@@ -16050,7 +16061,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -16207,7 +16218,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>45</v>
       </c>
@@ -16364,7 +16375,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -16521,7 +16532,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>47</v>
       </c>
@@ -16678,7 +16689,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>48</v>
       </c>
@@ -16835,7 +16846,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>49</v>
       </c>
@@ -16992,7 +17003,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>50</v>
       </c>
@@ -17149,7 +17160,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>51</v>
       </c>
@@ -17306,7 +17317,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>52</v>
       </c>
@@ -17463,7 +17474,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>53</v>
       </c>
@@ -17620,7 +17631,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>54</v>
       </c>
@@ -17777,7 +17788,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>55</v>
       </c>
@@ -17934,7 +17945,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>56</v>
       </c>
@@ -18091,7 +18102,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
@@ -18248,7 +18259,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>58</v>
       </c>
@@ -18405,7 +18416,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>59</v>
       </c>
@@ -18562,7 +18573,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>60</v>
       </c>
@@ -18719,7 +18730,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>61</v>
       </c>
@@ -18876,7 +18887,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>62</v>
       </c>
@@ -19033,7 +19044,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>63</v>
       </c>
@@ -19190,7 +19201,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>64</v>
       </c>
@@ -19347,7 +19358,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>65</v>
       </c>
@@ -19504,7 +19515,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>66</v>
       </c>
@@ -19661,7 +19672,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>67</v>
       </c>
@@ -19818,7 +19829,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>68</v>
       </c>
@@ -19975,7 +19986,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>69</v>
       </c>
@@ -20132,7 +20143,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>70</v>
       </c>
@@ -20289,7 +20300,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>71</v>
       </c>
@@ -20446,7 +20457,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>72</v>
       </c>
@@ -20603,7 +20614,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>73</v>
       </c>
@@ -20760,7 +20771,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>74</v>
       </c>
@@ -20917,7 +20928,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>75</v>
       </c>
@@ -21074,7 +21085,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>76</v>
       </c>
@@ -21231,7 +21242,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>77</v>
       </c>
@@ -21388,7 +21399,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>78</v>
       </c>
@@ -21545,7 +21556,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>79</v>
       </c>
@@ -21702,7 +21713,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>80</v>
       </c>
@@ -21859,7 +21870,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>81</v>
       </c>
@@ -22016,7 +22027,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>82</v>
       </c>
@@ -22184,30 +22195,30 @@
   <dimension ref="A1:CW55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AR25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="BL4" sqref="BL4:BL55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.08203125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.08203125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.08203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="64" width="11.08203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="64" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="65" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:101" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:101" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -22401,7 +22412,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -22558,7 +22569,7 @@
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
     </row>
-    <row r="5" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>32</v>
       </c>
@@ -22715,7 +22726,7 @@
       <c r="CV5" s="10"/>
       <c r="CW5" s="10"/>
     </row>
-    <row r="6" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -22872,7 +22883,7 @@
       <c r="CV6" s="10"/>
       <c r="CW6" s="10"/>
     </row>
-    <row r="7" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
@@ -23029,7 +23040,7 @@
       <c r="CV7" s="10"/>
       <c r="CW7" s="10"/>
     </row>
-    <row r="8" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>35</v>
       </c>
@@ -23186,7 +23197,7 @@
       <c r="CV8" s="10"/>
       <c r="CW8" s="10"/>
     </row>
-    <row r="9" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>36</v>
       </c>
@@ -23343,7 +23354,7 @@
       <c r="CV9" s="10"/>
       <c r="CW9" s="10"/>
     </row>
-    <row r="10" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -23500,7 +23511,7 @@
       <c r="CV10" s="10"/>
       <c r="CW10" s="10"/>
     </row>
-    <row r="11" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
@@ -23657,7 +23668,7 @@
       <c r="CV11" s="10"/>
       <c r="CW11" s="10"/>
     </row>
-    <row r="12" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>39</v>
       </c>
@@ -23814,7 +23825,7 @@
       <c r="CV12" s="10"/>
       <c r="CW12" s="10"/>
     </row>
-    <row r="13" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>40</v>
       </c>
@@ -23971,7 +23982,7 @@
       <c r="CV13" s="10"/>
       <c r="CW13" s="10"/>
     </row>
-    <row r="14" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>41</v>
       </c>
@@ -24128,7 +24139,7 @@
       <c r="CV14" s="10"/>
       <c r="CW14" s="10"/>
     </row>
-    <row r="15" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>42</v>
       </c>
@@ -24285,7 +24296,7 @@
       <c r="CV15" s="10"/>
       <c r="CW15" s="10"/>
     </row>
-    <row r="16" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>43</v>
       </c>
@@ -24442,7 +24453,7 @@
       <c r="CV16" s="10"/>
       <c r="CW16" s="10"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -24599,7 +24610,7 @@
       <c r="CV17" s="10"/>
       <c r="CW17" s="10"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>45</v>
       </c>
@@ -24756,7 +24767,7 @@
       <c r="CV18" s="10"/>
       <c r="CW18" s="10"/>
     </row>
-    <row r="19" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
@@ -24913,7 +24924,7 @@
       <c r="CV19" s="10"/>
       <c r="CW19" s="10"/>
     </row>
-    <row r="20" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>47</v>
       </c>
@@ -25070,7 +25081,7 @@
       <c r="CV20" s="10"/>
       <c r="CW20" s="10"/>
     </row>
-    <row r="21" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>48</v>
       </c>
@@ -25227,7 +25238,7 @@
       <c r="CV21" s="10"/>
       <c r="CW21" s="10"/>
     </row>
-    <row r="22" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>49</v>
       </c>
@@ -25384,7 +25395,7 @@
       <c r="CV22" s="10"/>
       <c r="CW22" s="10"/>
     </row>
-    <row r="23" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>50</v>
       </c>
@@ -25541,7 +25552,7 @@
       <c r="CV23" s="10"/>
       <c r="CW23" s="10"/>
     </row>
-    <row r="24" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>51</v>
       </c>
@@ -25698,7 +25709,7 @@
       <c r="CV24" s="10"/>
       <c r="CW24" s="10"/>
     </row>
-    <row r="25" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>52</v>
       </c>
@@ -25855,7 +25866,7 @@
       <c r="CV25" s="10"/>
       <c r="CW25" s="10"/>
     </row>
-    <row r="26" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>53</v>
       </c>
@@ -26012,7 +26023,7 @@
       <c r="CV26" s="10"/>
       <c r="CW26" s="10"/>
     </row>
-    <row r="27" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
         <v>54</v>
       </c>
@@ -26169,7 +26180,7 @@
       <c r="CV27" s="10"/>
       <c r="CW27" s="10"/>
     </row>
-    <row r="28" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>55</v>
       </c>
@@ -26326,7 +26337,7 @@
       <c r="CV28" s="10"/>
       <c r="CW28" s="10"/>
     </row>
-    <row r="29" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>56</v>
       </c>
@@ -26483,7 +26494,7 @@
       <c r="CV29" s="10"/>
       <c r="CW29" s="10"/>
     </row>
-    <row r="30" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>57</v>
       </c>
@@ -26640,7 +26651,7 @@
       <c r="CV30" s="10"/>
       <c r="CW30" s="10"/>
     </row>
-    <row r="31" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>58</v>
       </c>
@@ -26797,7 +26808,7 @@
       <c r="CV31" s="10"/>
       <c r="CW31" s="10"/>
     </row>
-    <row r="32" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>59</v>
       </c>
@@ -26954,7 +26965,7 @@
       <c r="CV32" s="10"/>
       <c r="CW32" s="10"/>
     </row>
-    <row r="33" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>60</v>
       </c>
@@ -27111,7 +27122,7 @@
       <c r="CV33" s="10"/>
       <c r="CW33" s="10"/>
     </row>
-    <row r="34" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>61</v>
       </c>
@@ -27268,7 +27279,7 @@
       <c r="CV34" s="10"/>
       <c r="CW34" s="10"/>
     </row>
-    <row r="35" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>62</v>
       </c>
@@ -27425,7 +27436,7 @@
       <c r="CV35" s="10"/>
       <c r="CW35" s="10"/>
     </row>
-    <row r="36" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>63</v>
       </c>
@@ -27582,7 +27593,7 @@
       <c r="CV36" s="10"/>
       <c r="CW36" s="10"/>
     </row>
-    <row r="37" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>64</v>
       </c>
@@ -27739,7 +27750,7 @@
       <c r="CV37" s="10"/>
       <c r="CW37" s="10"/>
     </row>
-    <row r="38" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>65</v>
       </c>
@@ -27896,7 +27907,7 @@
       <c r="CV38" s="10"/>
       <c r="CW38" s="10"/>
     </row>
-    <row r="39" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>66</v>
       </c>
@@ -28053,7 +28064,7 @@
       <c r="CV39" s="10"/>
       <c r="CW39" s="10"/>
     </row>
-    <row r="40" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>67</v>
       </c>
@@ -28210,7 +28221,7 @@
       <c r="CV40" s="10"/>
       <c r="CW40" s="10"/>
     </row>
-    <row r="41" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
         <v>68</v>
       </c>
@@ -28367,7 +28378,7 @@
       <c r="CV41" s="10"/>
       <c r="CW41" s="10"/>
     </row>
-    <row r="42" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
         <v>69</v>
       </c>
@@ -28524,7 +28535,7 @@
       <c r="CV42" s="10"/>
       <c r="CW42" s="10"/>
     </row>
-    <row r="43" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
         <v>70</v>
       </c>
@@ -28681,7 +28692,7 @@
       <c r="CV43" s="10"/>
       <c r="CW43" s="10"/>
     </row>
-    <row r="44" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>71</v>
       </c>
@@ -28838,7 +28849,7 @@
       <c r="CV44" s="10"/>
       <c r="CW44" s="10"/>
     </row>
-    <row r="45" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>72</v>
       </c>
@@ -28995,7 +29006,7 @@
       <c r="CV45" s="10"/>
       <c r="CW45" s="10"/>
     </row>
-    <row r="46" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
         <v>73</v>
       </c>
@@ -29152,7 +29163,7 @@
       <c r="CV46" s="10"/>
       <c r="CW46" s="10"/>
     </row>
-    <row r="47" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>74</v>
       </c>
@@ -29309,7 +29320,7 @@
       <c r="CV47" s="10"/>
       <c r="CW47" s="10"/>
     </row>
-    <row r="48" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
         <v>75</v>
       </c>
@@ -29466,7 +29477,7 @@
       <c r="CV48" s="10"/>
       <c r="CW48" s="10"/>
     </row>
-    <row r="49" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>76</v>
       </c>
@@ -29623,7 +29634,7 @@
       <c r="CV49" s="10"/>
       <c r="CW49" s="10"/>
     </row>
-    <row r="50" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A50" s="14" t="s">
         <v>77</v>
       </c>
@@ -29780,7 +29791,7 @@
       <c r="CV50" s="10"/>
       <c r="CW50" s="10"/>
     </row>
-    <row r="51" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A51" s="14" t="s">
         <v>78</v>
       </c>
@@ -29937,7 +29948,7 @@
       <c r="CV51" s="10"/>
       <c r="CW51" s="10"/>
     </row>
-    <row r="52" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
         <v>79</v>
       </c>
@@ -30094,7 +30105,7 @@
       <c r="CV52" s="10"/>
       <c r="CW52" s="10"/>
     </row>
-    <row r="53" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
         <v>80</v>
       </c>
@@ -30251,7 +30262,7 @@
       <c r="CV53" s="10"/>
       <c r="CW53" s="10"/>
     </row>
-    <row r="54" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
         <v>81</v>
       </c>
@@ -30408,7 +30419,7 @@
       <c r="CV54" s="10"/>
       <c r="CW54" s="10"/>
     </row>
-    <row r="55" spans="1:101" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
         <v>82</v>
       </c>

</xml_diff>